<commit_message>
Add kernel count image results output
</commit_message>
<xml_diff>
--- a/sample_test/5_ears_test/trait.xlsx
+++ b/sample_test/5_ears_test/trait.xlsx
@@ -508,28 +508,28 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>60.94697399198041</v>
+        <v>63.34496825573626</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9451466674660352</v>
+        <v>0.9427239224483256</v>
       </c>
       <c r="F2" t="n">
-        <v>5.178358208955224</v>
+        <v>5.299253731343284</v>
       </c>
       <c r="G2" t="n">
-        <v>14.91044776119403</v>
+        <v>15.47462686567164</v>
       </c>
       <c r="H2" t="n">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3060649470806985</v>
+        <v>0.2724400683851932</v>
       </c>
       <c r="J2" t="n">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2867875134166347</v>
+        <v>0.2628502434054487</v>
       </c>
       <c r="L2" t="n">
         <v>2.7</v>
@@ -556,28 +556,28 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>54.9437669859657</v>
+        <v>57.22118149922032</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9590303845358082</v>
+        <v>0.9581351127950248</v>
       </c>
       <c r="F3" t="n">
-        <v>4.835820895522389</v>
+        <v>4.956716417910448</v>
       </c>
       <c r="G3" t="n">
-        <v>14.7089552238806</v>
+        <v>14.85</v>
       </c>
       <c r="H3" t="n">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3275980409739817</v>
+        <v>0.2864291064666009</v>
       </c>
       <c r="J3" t="n">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3067402903679079</v>
+        <v>0.2555510866841167</v>
       </c>
       <c r="L3" t="n">
         <v>2.7</v>
@@ -604,28 +604,28 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>49.88794330585878</v>
+        <v>52.52100718422812</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9081169280348961</v>
+        <v>0.90365981393659</v>
       </c>
       <c r="F4" t="n">
-        <v>4.311940298507463</v>
+        <v>4.452985074626866</v>
       </c>
       <c r="G4" t="n">
-        <v>16.3410447761194</v>
+        <v>16.90522388059702</v>
       </c>
       <c r="H4" t="n">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2394210206144936</v>
+        <v>0.2070724859126186</v>
       </c>
       <c r="J4" t="n">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2593184349622309</v>
+        <v>0.1969933249530599</v>
       </c>
       <c r="L4" t="n">
         <v>2.7</v>
@@ -652,28 +652,28 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>40.52636695255069</v>
+        <v>42.56708788148809</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9067626389368917</v>
+        <v>0.91010710845327</v>
       </c>
       <c r="F5" t="n">
-        <v>4.352238805970149</v>
+        <v>4.452985074626866</v>
       </c>
       <c r="G5" t="n">
-        <v>11.58582089552239</v>
+        <v>11.76716417910448</v>
       </c>
       <c r="H5" t="n">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3565590888839386</v>
+        <v>0.2920866546947045</v>
       </c>
       <c r="J5" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3209971597237692</v>
+        <v>0.293265084492251</v>
       </c>
       <c r="L5" t="n">
         <v>2.7</v>
@@ -700,28 +700,28 @@
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>29.17826965916686</v>
+        <v>30.76062513922923</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7141396151330893</v>
+        <v>0.7182461905987475</v>
       </c>
       <c r="F6" t="n">
-        <v>3.606716417910448</v>
+        <v>3.707462686567164</v>
       </c>
       <c r="G6" t="n">
-        <v>11.14253731343284</v>
+        <v>11.2634328358209</v>
       </c>
       <c r="H6" t="n">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3666296148160149</v>
+        <v>0.2442220960415315</v>
       </c>
       <c r="J6" t="n">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3097999022863971</v>
+        <v>0.2420939835690309</v>
       </c>
       <c r="L6" t="n">
         <v>2.7</v>

</xml_diff>